<commit_message>
added new column-remarks to inquiry item table and changed code according to that
</commit_message>
<xml_diff>
--- a/uploads/inquiries/Inquiry_1.xlsx
+++ b/uploads/inquiries/Inquiry_1.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Inquiry_4" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Inquiry_1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="Ms1mQQBBT+qAsdblTxwpTS2fx6d9ell4dMIswkrQLfg="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="IUrbwaZGN1hIWicfCf0tKJKbHL9aOJPBe1NSWHRegqE="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Product Name</t>
   </si>
@@ -36,16 +36,22 @@
     <t>Status</t>
   </si>
   <si>
-    <t>biscuits</t>
+    <t>Sugar 5kg</t>
   </si>
   <si>
     <t>Available</t>
   </si>
   <si>
-    <t>Sugar 5kg</t>
+    <t>biscuits</t>
   </si>
   <si>
-    <t>test</t>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>we only have 5 kg</t>
   </si>
 </sst>
 </file>
@@ -315,8 +321,9 @@
     <col customWidth="1" min="3" max="3" width="10.0"/>
     <col customWidth="1" min="4" max="4" width="9.14"/>
     <col customWidth="1" min="5" max="5" width="13.71"/>
-    <col customWidth="1" min="6" max="6" width="13.0"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col customWidth="1" min="6" max="6" width="19.43"/>
+    <col customWidth="1" min="7" max="7" width="22.57"/>
+    <col customWidth="1" min="8" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -344,16 +351,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="2">
-        <v>20.0</v>
+        <v>50.0</v>
       </c>
       <c r="C2" s="3">
-        <v>100.0</v>
+        <v>200.0</v>
       </c>
       <c r="D2" s="2">
         <v>0.0</v>
       </c>
       <c r="E2" s="3">
-        <v>2000.0</v>
+        <v>10000.0</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>7</v>
@@ -364,16 +371,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>10.0</v>
+        <v>30.0</v>
       </c>
       <c r="C3" s="3">
-        <v>200.0</v>
+        <v>150.0</v>
       </c>
       <c r="D3" s="2">
         <v>0.0</v>
       </c>
       <c r="E3" s="3">
-        <v>2000.0</v>
+        <v>4500.0</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
@@ -387,16 +394,19 @@
         <v>10.0</v>
       </c>
       <c r="C4" s="3">
-        <v>150.0</v>
+        <v>1000.0</v>
       </c>
       <c r="D4" s="2">
         <v>0.0</v>
       </c>
-      <c r="E4" s="3">
-        <v>1500.0</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>7</v>
+      <c r="E4" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
update inquiry service impl missing code
</commit_message>
<xml_diff>
--- a/uploads/inquiries/Inquiry_1.xlsx
+++ b/uploads/inquiries/Inquiry_1.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="IUrbwaZGN1hIWicfCf0tKJKbHL9aOJPBe1NSWHRegqE="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="h4y4aTKVyAuxPlIJBNrVVt0pPz39TOcryfEqzarIyJg="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Product Name</t>
   </si>
@@ -27,31 +27,22 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Total Amount</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Sugar 5kg</t>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Chicken</t>
   </si>
   <si>
     <t>Available</t>
   </si>
   <si>
-    <t>biscuits</t>
+    <t/>
   </si>
   <si>
-    <t>Chicken</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>we only have 5 kg</t>
+    <t>Beef</t>
   </si>
 </sst>
 </file>
@@ -319,11 +310,9 @@
     <col customWidth="1" min="1" max="1" width="14.14"/>
     <col customWidth="1" min="2" max="2" width="9.14"/>
     <col customWidth="1" min="3" max="3" width="10.0"/>
-    <col customWidth="1" min="4" max="4" width="9.14"/>
-    <col customWidth="1" min="5" max="5" width="13.71"/>
-    <col customWidth="1" min="6" max="6" width="19.43"/>
-    <col customWidth="1" min="7" max="7" width="22.57"/>
-    <col customWidth="1" min="8" max="26" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="20.29"/>
+    <col customWidth="1" min="5" max="5" width="8.14"/>
+    <col customWidth="1" min="6" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -342,27 +331,21 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>850.0</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>200.0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="3">
-        <v>10000.0</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -371,42 +354,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>30.0</v>
+        <v>10.0</v>
       </c>
       <c r="C3" s="3">
-        <v>150.0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>4500.0</v>
-      </c>
-      <c r="F3" s="3" t="s">
+        <v>2600.0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2">
-        <v>10.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1000.0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add functionality to retrieve confirmed inquiries and display confirmation descriptions
</commit_message>
<xml_diff>
--- a/uploads/inquiries/Inquiry_1.xlsx
+++ b/uploads/inquiries/Inquiry_1.xlsx
@@ -7,16 +7,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="h4y4aTKVyAuxPlIJBNrVVt0pPz39TOcryfEqzarIyJg="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Product Name</t>
   </si>
@@ -33,7 +28,7 @@
     <t>Remark</t>
   </si>
   <si>
-    <t>Chicken</t>
+    <t>PASTA SAUCE-350 GRM</t>
   </si>
   <si>
     <t>Available</t>
@@ -42,7 +37,16 @@
     <t/>
   </si>
   <si>
-    <t>Beef</t>
+    <t>FISH SAUCE-600 ML</t>
+  </si>
+  <si>
+    <t>PRIMA KOTTU MEE - 80GRM</t>
+  </si>
+  <si>
+    <t>PIZZA BASE-5 PCS</t>
+  </si>
+  <si>
+    <t>There is a 10% discount for 20+</t>
   </si>
 </sst>
 </file>
@@ -307,11 +311,11 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.14"/>
+    <col customWidth="1" min="1" max="1" width="26.57"/>
     <col customWidth="1" min="2" max="2" width="9.14"/>
     <col customWidth="1" min="3" max="3" width="10.0"/>
-    <col customWidth="1" min="4" max="4" width="20.29"/>
-    <col customWidth="1" min="5" max="5" width="8.14"/>
+    <col customWidth="1" min="4" max="4" width="18.86"/>
+    <col customWidth="1" min="5" max="5" width="42.71"/>
     <col customWidth="1" min="6" max="26" width="8.71"/>
   </cols>
   <sheetData>
@@ -337,7 +341,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>10.0</v>
+        <v>15.0</v>
       </c>
       <c r="C2" s="3">
         <v>850.0</v>
@@ -345,7 +349,7 @@
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -357,13 +361,47 @@
         <v>10.0</v>
       </c>
       <c r="C3" s="3">
-        <v>2600.0</v>
+        <v>600.0</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>140.0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>30.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>850.0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>